<commit_message>
2017-06-27: 1. rule done 2. mongo db define done
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="global_config" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="inputRule" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -31,7 +31,61 @@
             <charset val="134"/>
           </rPr>
           <t>zw:
-对浏览器传入的值的定义</t>
+对inputRule的值的定义(cilent和server的字段合并在一起，方便操作)。每个字段的rule间隔2（以便可以插入新rule）。下一个Coll的rc以10为单位取整，以便如果有新字段加入，还有rc可以那个</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>和</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>inputRule</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>一致，只是开头改成</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>2</t>
         </r>
       </text>
     </comment>
@@ -172,8 +226,96 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ZHANG Wei AG</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>ZHANG Wei AG:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>上一个</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>coll</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>正好以</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>10</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>的整数结尾，所以</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
+          </rPr>
+          <t>+10</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>后起始</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112">
   <si>
     <t>rc</t>
   </si>
@@ -224,10 +366,76 @@
     <t>serverMsg</t>
   </si>
   <si>
-    <t>inputFromClient</t>
-  </si>
-  <si>
-    <t>10000-10999</t>
+    <t>inputRule</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>10000-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>999</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ongoRule</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0000-29999</t>
+    </r>
   </si>
   <si>
     <t>inputGenerateByServer</t>
@@ -254,25 +462,103 @@
     <t>runtime_node_error</t>
   </si>
   <si>
-    <t>12000-12999</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0000～49999</t>
+    </r>
   </si>
   <si>
     <t>validate_helper</t>
   </si>
   <si>
-    <t>12000-12299</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>40000-400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>99</t>
+    </r>
   </si>
   <si>
     <t>validate_format</t>
   </si>
   <si>
-    <t>12300-12599</t>
+    <t>40100-40199</t>
   </si>
   <si>
     <t>validate_value</t>
   </si>
   <si>
-    <t>12600-12899</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>402</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>99</t>
+    </r>
   </si>
   <si>
     <t>60000-68999</t>
@@ -388,25 +674,406 @@
     <t>mongoose_operation_error</t>
   </si>
   <si>
-    <t>32000-32999</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>000-3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>999</t>
+    </r>
   </si>
   <si>
     <t>runtime_es_error</t>
   </si>
   <si>
-    <t>33000-33999</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>000-3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>999</t>
+    </r>
   </si>
   <si>
     <t>runtime_redis_error</t>
   </si>
   <si>
-    <t>34000-34999</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>000-3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>999</t>
+    </r>
   </si>
   <si>
     <t>imageDefine</t>
   </si>
   <si>
     <t>uploadDefine</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>dmin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>dmin_user</t>
+    </r>
+  </si>
+  <si>
+    <t>10000~10030</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>dmin_sugar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0030~10040</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ategory</t>
+    </r>
+  </si>
+  <si>
+    <t>10050~10060</t>
+  </si>
+  <si>
+    <t>store_path</t>
+  </si>
+  <si>
+    <t>10060~10070</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rticle</t>
+    </r>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>10100~10170</t>
+  </si>
+  <si>
+    <t>article_comment</t>
+  </si>
+  <si>
+    <t>10170~10190</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>10190~10210</t>
+  </si>
+  <si>
+    <t>like_dislike</t>
+  </si>
+  <si>
+    <t>10210~10220</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>10220~10230</t>
+  </si>
+  <si>
+    <t>article_attachment</t>
+  </si>
+  <si>
+    <t>10230~10260</t>
+  </si>
+  <si>
+    <t>article_image</t>
+  </si>
+  <si>
+    <t>10260~10300</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>member_penalize</t>
+  </si>
+  <si>
+    <t>10300~10330</t>
+  </si>
+  <si>
+    <t>public_group</t>
+  </si>
+  <si>
+    <t>10330~10360</t>
+  </si>
+  <si>
+    <t>public_group_event</t>
+  </si>
+  <si>
+    <t>10360~10390</t>
+  </si>
+  <si>
+    <t>public_group_interaction</t>
+  </si>
+  <si>
+    <t>10390~10410</t>
+  </si>
+  <si>
+    <t>user_friend_group</t>
+  </si>
+  <si>
+    <t>10410~10430</t>
+  </si>
+  <si>
+    <t>user+public_group</t>
+  </si>
+  <si>
+    <t>10430~10440</t>
+  </si>
+  <si>
+    <t>impeach</t>
+  </si>
+  <si>
+    <t>10500~10560</t>
+  </si>
+  <si>
+    <t>impeach_comment</t>
+  </si>
+  <si>
+    <t>10560~10590</t>
+  </si>
+  <si>
+    <t>impeach_dealer</t>
+  </si>
+  <si>
+    <t>10590~10610</t>
+  </si>
+  <si>
+    <t>impeach_image</t>
+  </si>
+  <si>
+    <t>10610~10640</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>10700~10740</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>10740~10760</t>
   </si>
 </sst>
 </file>
@@ -414,12 +1081,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -434,8 +1107,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,31 +1158,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,23 +1203,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,10 +1219,34 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -533,51 +1258,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -594,187 +1274,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,11 +1483,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,17 +1528,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -856,30 +1560,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -890,163 +1570,167 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1436,7 +2120,6 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1445,8 +2128,8 @@
   <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1483,265 +2166,271 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="3:3">
-      <c r="C3" s="4"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="3:4">
-      <c r="C5" s="4" t="s">
-        <v>9</v>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="2:4">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="2:4">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8">
         <v>20000</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="3:3">
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="3:3">
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="3:3">
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" ht="14" customHeight="1" spans="2:4">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" ht="14" customHeight="1" spans="2:4">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" ht="14.1" customHeight="1" spans="2:4">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" ht="14" customHeight="1" spans="2:4">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+    <row r="13" ht="14.1" customHeight="1" spans="2:4">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="14" ht="14.1" customHeight="1" spans="2:4">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="4"/>
+      <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="4"/>
+      <c r="B19" s="5"/>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>34</v>
+      <c r="B21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="4"/>
-      <c r="E22" s="4" t="s">
-        <v>36</v>
+      <c r="B22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>38</v>
+      <c r="B23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="4"/>
-      <c r="E24" s="4" t="s">
-        <v>40</v>
+      <c r="B24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
+      <c r="B25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="4"/>
-      <c r="E27" s="7" t="s">
-        <v>44</v>
+      <c r="B27" s="5"/>
+      <c r="E27" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="4">
+        <v>48</v>
+      </c>
+      <c r="B28" s="5">
         <v>70000</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" s="3" customFormat="1" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="7">
+        <v>49</v>
+      </c>
+      <c r="B29" s="9">
         <v>80000</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>50</v>
+      <c r="A33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>52</v>
+      <c r="A34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1765,7 +2454,7 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>50000</v>
@@ -1773,7 +2462,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>50100</v>
@@ -1788,15 +2477,220 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A2:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="27.125" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-07-12: 1. register add roll back like logic; 2. register API test done
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -53,7 +53,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -70,7 +70,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -86,7 +86,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>2</t>
         </r>
@@ -242,7 +242,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -250,7 +250,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -267,7 +267,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -283,7 +283,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>10</t>
         </r>
@@ -299,7 +299,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
   <si>
     <t>rc</t>
   </si>
@@ -1205,19 +1205,21 @@
   </si>
   <si>
     <t>32000~33000</t>
+  </si>
+  <si>
+    <t>mongo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>30000~31000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1239,352 +1241,37 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1592,251 +1279,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1858,57 +1303,10 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2241,19 +1639,19 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.375" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
@@ -2263,7 +1661,7 @@
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +1678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2289,7 +1687,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2298,7 +1696,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2307,7 +1705,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2315,7 +1713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" spans="2:4">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
         <v>13</v>
@@ -2324,7 +1722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:3">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2333,16 +1731,16 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2351,7 +1749,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" ht="14.1" customHeight="1" spans="2:4">
+    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -2360,7 +1758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" ht="14.1" customHeight="1" spans="2:4">
+    <row r="13" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -2369,7 +1767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" ht="14.1" customHeight="1" spans="2:4">
+    <row r="14" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -2378,15 +1776,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2400,48 +1798,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="2:5">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="2:6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="2:5">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B27" s="1"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2450,7 +1845,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:3">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -2459,12 +1854,12 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -2472,7 +1867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
@@ -2480,7 +1875,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2488,7 +1883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -2496,7 +1891,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2505,28 +1900,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2534,7 +1928,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -2543,28 +1937,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -2575,7 +1968,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
@@ -2583,7 +1976,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
@@ -2591,7 +1984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2599,7 +1992,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
@@ -2607,7 +2000,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1" spans="1:3">
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -2618,7 +2011,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>57</v>
       </c>
@@ -2626,7 +2019,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>59</v>
       </c>
@@ -2634,7 +2027,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>61</v>
       </c>
@@ -2642,7 +2035,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -2650,7 +2043,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>65</v>
       </c>
@@ -2658,7 +2051,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>67</v>
       </c>
@@ -2666,7 +2059,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>61</v>
       </c>
@@ -2674,11 +2067,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
     </row>
-    <row r="17" ht="12.75" customHeight="1"/>
-    <row r="18" spans="1:3">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2689,7 +2082,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>73</v>
       </c>
@@ -2697,7 +2090,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -2705,7 +2098,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -2713,7 +2106,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -2721,7 +2114,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>81</v>
       </c>
@@ -2729,7 +2122,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -2740,7 +2133,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>85</v>
       </c>
@@ -2748,7 +2141,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>87</v>
       </c>
@@ -2756,7 +2149,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>89</v>
       </c>
@@ -2764,7 +2157,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -2775,7 +2168,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>93</v>
       </c>
@@ -2783,7 +2176,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>95</v>
       </c>
@@ -2794,7 +2187,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
         <v>98</v>
       </c>
@@ -2802,7 +2195,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>100</v>
       </c>
@@ -2811,29 +2204,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -2844,7 +2236,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2852,7 +2244,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2860,7 +2252,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2869,7 +2261,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -2877,7 +2269,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -2885,7 +2277,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -2893,7 +2285,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -2902,27 +2294,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -2936,7 +2327,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>120</v>
       </c>
@@ -2944,12 +2335,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="4:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2958,33 +2349,38 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A2:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>124</v>
       </c>
+      <c r="G2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20170717: add test case for unique check in register
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" activeTab="5"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -53,7 +53,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -70,7 +70,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -86,7 +86,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>2</t>
         </r>
@@ -242,7 +242,7 @@
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -250,7 +250,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -267,7 +267,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -283,7 +283,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>10</t>
         </r>
@@ -299,7 +299,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
   <si>
     <t>rc</t>
   </si>
@@ -665,6 +665,15 @@
     <t>50000~50100</t>
   </si>
   <si>
+    <t>user-register</t>
+  </si>
+  <si>
+    <t>50100~50200</t>
+  </si>
+  <si>
+    <t>rest api的error直接写在controller文件中</t>
+  </si>
+  <si>
     <t>global_config</t>
   </si>
   <si>
@@ -1208,18 +1217,22 @@
   </si>
   <si>
     <t>mongo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>30000~31000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1241,37 +1254,352 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1279,9 +1607,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1303,10 +1873,57 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1639,29 +2256,29 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="30.375" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
     <col min="3" max="3" width="17.125" customWidth="1"/>
     <col min="4" max="4" width="29.375" customWidth="1"/>
     <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="42.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +2295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1687,7 +2304,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1696,7 +2313,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1705,7 +2322,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="3:4">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1713,7 +2330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" s="3" customFormat="1" spans="2:4">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
         <v>13</v>
@@ -1722,7 +2339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" s="3" customFormat="1" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1731,16 +2348,16 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="3:3">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="3:3">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="3:3">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1749,7 +2366,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" ht="14.1" customHeight="1" spans="2:4">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1758,7 +2375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" ht="14.1" customHeight="1" spans="2:4">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -1767,7 +2384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" ht="14.1" customHeight="1" spans="2:4">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -1776,15 +2393,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1798,549 +2415,565 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:6">
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:6">
       <c r="B21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:6">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:6">
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:5">
       <c r="B27" s="1"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1">
         <v>70000</v>
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" s="2" customFormat="1" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B29" s="4">
         <v>80000</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>50100</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="27.125" customWidth="1"/>
     <col min="3" max="3" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
       <c r="C14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
       <c r="B15" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" ht="12.75" customHeight="1"/>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
       <c r="B35" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4">
       <c r="C3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2349,38 +2982,39 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-07-29: 1. upload user photo chose save dir automatically
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\express\doc\错误代码\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,14 +43,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1">
+    <comment ref="A3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -53,7 +58,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -70,7 +75,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -86,13 +91,13 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>2</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="1">
+    <comment ref="F21" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1">
+    <comment ref="F22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1">
+    <comment ref="F24" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="1">
+    <comment ref="F25" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0">
+    <comment ref="A28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0">
+    <comment ref="A29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0">
+    <comment ref="A36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0">
+    <comment ref="A37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -235,14 +240,14 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -250,7 +255,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -267,7 +272,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -283,7 +288,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>10</t>
         </r>
@@ -299,7 +304,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -323,7 +328,7 @@
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -358,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -407,7 +412,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
   <si>
     <t>rc</t>
   </si>
@@ -960,15 +965,9 @@
     <t>store_path</t>
   </si>
   <si>
-    <t>10060~10070</t>
-  </si>
-  <si>
     <t>admin_penalize</t>
   </si>
   <si>
-    <t>10070~10100</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1186,53 +1185,105 @@
     <t>misc</t>
   </si>
   <si>
+    <t>mongodb</t>
+  </si>
+  <si>
+    <t>mongoError</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>30000~30099</t>
+  </si>
+  <si>
+    <t>err.errors</t>
+  </si>
+  <si>
+    <t>inputRule=&gt;validator</t>
+  </si>
+  <si>
+    <t>30100～30199</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>32000~33000</t>
+  </si>
+  <si>
+    <t>mongo</t>
+  </si>
+  <si>
+    <t>30000~31000</t>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50000~50100</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50100~50200</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>article</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>50200~50300</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10060~10080</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0~10100</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>40800~40900</t>
-  </si>
-  <si>
-    <t>mongodb</t>
-  </si>
-  <si>
-    <t>mongoError</t>
-  </si>
-  <si>
-    <t>common</t>
-  </si>
-  <si>
-    <t>30000~30099</t>
-  </si>
-  <si>
-    <t>err.errors</t>
-  </si>
-  <si>
-    <t>inputRule=&gt;validator</t>
-  </si>
-  <si>
-    <t>30100～30199</t>
-  </si>
-  <si>
-    <t>redis</t>
-  </si>
-  <si>
-    <t>32000~33000</t>
-  </si>
-  <si>
-    <t>mongo</t>
-  </si>
-  <si>
-    <t>30000~31000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>system</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>40900~41000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1254,352 +1305,44 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="8"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1607,255 +1350,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1872,62 +1373,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2256,29 +1714,29 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.375" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="29.375" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
-    <col min="6" max="6" width="42.625" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="4" max="4" width="29.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="42.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2304,7 +1762,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2313,7 +1771,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2322,7 +1780,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2330,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" spans="2:4">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
         <v>13</v>
@@ -2339,7 +1797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:3">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2348,16 +1806,16 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2366,7 +1824,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" ht="14.1" customHeight="1" spans="2:4">
+    <row r="12" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -2375,7 +1833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" ht="14.1" customHeight="1" spans="2:4">
+    <row r="13" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -2384,7 +1842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" ht="14.1" customHeight="1" spans="2:4">
+    <row r="14" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -2393,15 +1851,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2415,7 +1873,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" t="s">
         <v>28</v>
@@ -2427,45 +1885,42 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="2:5">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="2:6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="2:5">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +1929,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:3">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2483,12 +1938,12 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
@@ -2496,7 +1951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -2504,7 +1959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2512,7 +1967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2520,7 +1975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2529,28 +1984,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2558,7 +2012,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2567,28 +2021,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.25" customWidth="1"/>
-    <col min="2" max="2" width="27.125" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -2599,7 +2052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2607,7 +2060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2615,406 +2068,428 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="C7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>58</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
-      <c r="B10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>64</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="17" ht="12.75" customHeight="1"/>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>74</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>76</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
-      <c r="B20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>78</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>80</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>84</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
-      <c r="B26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>90</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>92</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>94</v>
       </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
-      <c r="B31" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B33" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="2" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A2:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="17.25" customWidth="1"/>
-    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>111</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>113</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A2:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
         <v>119</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>120</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>121</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="4:4">
-      <c r="D4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" t="s">
-        <v>129</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-08-12: 1. optimze CRUD precedure 2. split article precedure 3. finish comment/likeDislike/uploadFile of article
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\express\doc\错误代码\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="12630" activeTab="3"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -30,7 +25,7 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,14 +38,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0">
+    <comment ref="A3" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -58,7 +53,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -75,7 +70,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -91,13 +86,13 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>2</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="1" shapeId="0">
+    <comment ref="F21" authorId="1">
       <text>
         <r>
           <rPr>
@@ -137,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1" shapeId="0">
+    <comment ref="F22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -150,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1" shapeId="0">
+    <comment ref="F24" authorId="1">
       <text>
         <r>
           <rPr>
@@ -163,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="1" shapeId="0">
+    <comment ref="F25" authorId="1">
       <text>
         <r>
           <rPr>
@@ -176,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0">
+    <comment ref="A28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0">
+    <comment ref="A29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0">
+    <comment ref="A37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -240,14 +235,14 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -255,7 +250,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -272,7 +267,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -288,7 +283,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>10</t>
         </r>
@@ -304,7 +299,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -328,7 +323,7 @@
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -363,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -412,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147">
   <si>
     <t>rc</t>
   </si>
@@ -965,6 +960,9 @@
     <t>store_path</t>
   </si>
   <si>
+    <t>10060~10080</t>
+  </si>
+  <si>
     <t>admin_penalize</t>
   </si>
   <si>
@@ -975,6 +973,44 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0~10100</t>
+    </r>
+  </si>
+  <si>
+    <t>resource_profile</t>
+  </si>
+  <si>
+    <t>11100~11200</t>
+  </si>
+  <si>
+    <t>code使用完毕，直接从user_operation=&gt;collection往后推</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>a</t>
     </r>
     <r>
@@ -1030,9 +1066,6 @@
     <t>10260~10290</t>
   </si>
   <si>
-    <t>10290~10300</t>
-  </si>
-  <si>
     <t>friend</t>
   </si>
   <si>
@@ -1146,6 +1179,24 @@
     <t>10860~10890</t>
   </si>
   <si>
+    <t>statci</t>
+  </si>
+  <si>
+    <t>like_dislike_static</t>
+  </si>
+  <si>
+    <t>11200~11210</t>
+  </si>
+  <si>
+    <t>resource_profile占用了11100~11200</t>
+  </si>
+  <si>
+    <t>resource_profile_static</t>
+  </si>
+  <si>
+    <t>11210~11230</t>
+  </si>
+  <si>
     <t>validate</t>
   </si>
   <si>
@@ -1185,6 +1236,15 @@
     <t>misc</t>
   </si>
   <si>
+    <t>40800~40900</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>40900~41000</t>
+  </si>
+  <si>
     <t>mongodb</t>
   </si>
   <si>
@@ -1206,6 +1266,27 @@
     <t>30100～30199</t>
   </si>
   <si>
+    <t>50200~50300</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>50300~50400</t>
+  </si>
+  <si>
+    <t>uploadFile</t>
+  </si>
+  <si>
+    <t>50400~50500</t>
+  </si>
+  <si>
+    <t>likeDislike</t>
+  </si>
+  <si>
+    <t>50500~50600</t>
+  </si>
+  <si>
     <t>redis</t>
   </si>
   <si>
@@ -1216,74 +1297,25 @@
   </si>
   <si>
     <t>30000~31000</t>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>50000~50100</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>50100~50200</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>article</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>50200~50300</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10060~10080</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0~10100</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>40800~40900</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>system</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>40900~41000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1305,44 +1337,352 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1350,9 +1690,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1362,30 +1944,74 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1714,29 +2340,29 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
-    <col min="4" max="4" width="29.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="42.6328125" customWidth="1"/>
+    <col min="1" max="1" width="30.3666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6333333333333" customWidth="1"/>
+    <col min="3" max="3" width="17.0916666666667" customWidth="1"/>
+    <col min="4" max="4" width="29.3666666666667" customWidth="1"/>
+    <col min="5" max="5" width="12.6333333333333" customWidth="1"/>
+    <col min="6" max="6" width="42.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1753,16 +2379,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1771,16 +2397,16 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1788,43 +2414,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+    <row r="6" s="4" customFormat="1" spans="2:4">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="4" customFormat="1" spans="1:3">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>20000</v>
       </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="3:3">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:3">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:3">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" ht="14.15" customHeight="1" spans="2:4">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1833,7 +2459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" ht="14.15" customHeight="1" spans="2:4">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -1842,7 +2468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" ht="14.15" customHeight="1" spans="2:4">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -1851,15 +2477,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1873,7 +2499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="1"/>
       <c r="C18" t="s">
         <v>28</v>
@@ -1885,42 +2511,45 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:5">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="1"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1929,82 +2558,83 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" s="2" customFormat="1" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="5">
         <v>80000</v>
       </c>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.9083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2012,7 +2642,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2021,27 +2651,28 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.2666666666667" customWidth="1"/>
+    <col min="2" max="2" width="27.0916666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -2052,7 +2683,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2060,7 +2691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2068,113 +2699,104 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="8" spans="2:3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" spans="1:3">
+      <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="C9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C15" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" ht="12.75" customHeight="1"/>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>76</v>
       </c>
@@ -2182,7 +2804,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>78</v>
       </c>
@@ -2190,7 +2812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>80</v>
       </c>
@@ -2198,7 +2820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>82</v>
       </c>
@@ -2206,26 +2828,26 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
         <v>84</v>
       </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
       <c r="B27" t="s">
         <v>88</v>
       </c>
@@ -2233,7 +2855,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>90</v>
       </c>
@@ -2241,45 +2863,45 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
         <v>92</v>
       </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="C33" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>101</v>
       </c>
@@ -2287,209 +2909,277 @@
         <v>102</v>
       </c>
     </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.45" customWidth="1"/>
+    <col min="2" max="2" width="17.2666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.725" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="2" max="3" width="11.45" customWidth="1"/>
+    <col min="4" max="4" width="22.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4">
       <c r="C3" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="H2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-08-15: functionalize image in content check
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\express\doc\错误代码\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -25,7 +30,7 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,14 +43,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1">
+    <comment ref="A3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -53,7 +58,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -70,7 +75,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -86,13 +91,13 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>2</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="1">
+    <comment ref="F21" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1">
+    <comment ref="F22" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1">
+    <comment ref="F24" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="1">
+    <comment ref="F25" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0">
+    <comment ref="A28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0">
+    <comment ref="A29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0">
+    <comment ref="A36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0">
+    <comment ref="A37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -235,14 +240,14 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -250,7 +255,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -267,7 +272,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -283,7 +288,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>10</t>
         </r>
@@ -299,7 +304,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -323,7 +328,7 @@
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -358,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -407,7 +412,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
   <si>
     <t>rc</t>
   </si>
@@ -1302,14 +1307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1337,352 +1336,37 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1690,251 +1374,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1957,61 +1399,17 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2340,29 +1738,29 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.3666666666667" customWidth="1"/>
-    <col min="2" max="2" width="12.6333333333333" customWidth="1"/>
-    <col min="3" max="3" width="17.0916666666667" customWidth="1"/>
-    <col min="4" max="4" width="29.3666666666667" customWidth="1"/>
-    <col min="5" max="5" width="12.6333333333333" customWidth="1"/>
-    <col min="6" max="6" width="42.6333333333333" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" customWidth="1"/>
+    <col min="4" max="4" width="29.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="42.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +1777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2388,7 +1786,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2397,7 +1795,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -2406,7 +1804,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -2414,7 +1812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" spans="2:4">
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -2423,7 +1821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" s="4" customFormat="1" spans="1:3">
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2432,16 +1830,16 @@
       </c>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2450,7 +1848,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" ht="14.15" customHeight="1" spans="2:4">
+    <row r="12" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -2459,7 +1857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" ht="14.15" customHeight="1" spans="2:4">
+    <row r="13" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -2468,7 +1866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" ht="14.15" customHeight="1" spans="2:4">
+    <row r="14" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -2477,15 +1875,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2499,7 +1897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" t="s">
         <v>28</v>
@@ -2511,45 +1909,42 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="2:5">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="2:6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="2:5">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2558,7 +1953,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:3">
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2567,12 +1962,12 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
@@ -2580,7 +1975,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
@@ -2588,7 +1983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2596,7 +1991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2604,7 +1999,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2613,28 +2008,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.9083333333333" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2642,7 +2036,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2651,28 +2045,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.2666666666667" customWidth="1"/>
-    <col min="2" max="2" width="27.0916666666667" customWidth="1"/>
-    <col min="3" max="3" width="12.6333333333333" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -2683,7 +2076,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2691,7 +2084,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2699,7 +2092,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2707,7 +2100,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>55</v>
       </c>
@@ -2715,7 +2108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>57</v>
       </c>
@@ -2726,11 +2119,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" ht="12.75" customHeight="1" spans="1:3">
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -2741,7 +2134,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>63</v>
       </c>
@@ -2749,7 +2142,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>65</v>
       </c>
@@ -2757,7 +2150,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -2765,7 +2158,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>69</v>
       </c>
@@ -2773,7 +2166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -2781,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -2789,11 +2182,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1"/>
-    <row r="20" spans="1:3">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2804,7 +2197,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>78</v>
       </c>
@@ -2812,7 +2205,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>80</v>
       </c>
@@ -2820,7 +2213,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>82</v>
       </c>
@@ -2828,7 +2221,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -2836,7 +2229,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>86</v>
       </c>
@@ -2844,7 +2237,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2855,7 +2248,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>90</v>
       </c>
@@ -2863,7 +2256,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>92</v>
       </c>
@@ -2871,7 +2264,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>94</v>
       </c>
@@ -2879,7 +2272,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -2890,7 +2283,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>98</v>
       </c>
@@ -2898,7 +2291,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -2909,7 +2302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>103</v>
       </c>
@@ -2917,7 +2310,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>105</v>
       </c>
@@ -2925,7 +2318,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2939,7 +2332,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>111</v>
       </c>
@@ -2948,30 +2341,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.45" customWidth="1"/>
-    <col min="2" max="2" width="17.2666666666667" customWidth="1"/>
-    <col min="3" max="3" width="12.725" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -2982,7 +2374,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2990,7 +2382,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2998,7 +2390,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -3007,7 +2399,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -3015,7 +2407,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3023,7 +2415,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -3031,7 +2423,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>125</v>
       </c>
@@ -3039,7 +2431,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -3048,27 +2440,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.45" customWidth="1"/>
-    <col min="4" max="4" width="22.6333333333333" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -3082,7 +2473,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>133</v>
       </c>
@@ -3090,12 +2481,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="4:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -3103,7 +2494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -3111,7 +2502,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -3122,7 +2513,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>137</v>
       </c>
@@ -3130,7 +2521,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>139</v>
       </c>
@@ -3138,7 +2529,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>141</v>
       </c>
@@ -3147,24 +2538,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -3179,7 +2569,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2017-08-23: 1. create impeach done  2. prepare test case for helper
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
   <si>
     <t>rc</t>
   </si>
@@ -1280,35 +1280,153 @@
     <t>50300~50400</t>
   </si>
   <si>
+    <t>50400~50500</t>
+  </si>
+  <si>
+    <t>likeDislike</t>
+  </si>
+  <si>
+    <t>50500~50600</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>32000~33000</t>
+  </si>
+  <si>
+    <t>mongo</t>
+  </si>
+  <si>
+    <t>30000~31000</t>
+  </si>
+  <si>
+    <t>impeach</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>uploadFile</t>
-  </si>
-  <si>
-    <t>50400~50500</t>
-  </si>
-  <si>
-    <t>likeDislike</t>
-  </si>
-  <si>
-    <t>50500~50600</t>
-  </si>
-  <si>
-    <t>redis</t>
-  </si>
-  <si>
-    <t>32000~33000</t>
-  </si>
-  <si>
-    <t>mongo</t>
-  </si>
-  <si>
-    <t>30000~31000</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50700</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>507</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>508</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1357,6 +1475,13 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1380,7 +1505,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1398,6 +1523,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2054,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -2447,10 +2573,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2523,18 +2649,45 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
         <v>139</v>
-      </c>
-      <c r="C21" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
         <v>141</v>
       </c>
-      <c r="C22" t="s">
-        <v>142</v>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2556,16 +2709,16 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>144</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>145</v>
-      </c>
-      <c r="H2" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017-09-24: 1. split down  2. ready to test admin_user
</commit_message>
<xml_diff>
--- a/express/doc/错误代码/错误代码范围.xlsx
+++ b/express/doc/错误代码/错误代码范围.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ss_vue_express\express\doc\错误代码\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050" activeTab="4"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -30,7 +25,7 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,14 +38,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="1" shapeId="0">
+    <comment ref="A3" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -58,7 +53,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -75,7 +70,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>inputRule</t>
         </r>
@@ -91,13 +86,13 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>2</t>
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="1" shapeId="0">
+    <comment ref="F21" authorId="1">
       <text>
         <r>
           <rPr>
@@ -137,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="1" shapeId="0">
+    <comment ref="F22" authorId="1">
       <text>
         <r>
           <rPr>
@@ -150,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1" shapeId="0">
+    <comment ref="F24" authorId="1">
       <text>
         <r>
           <rPr>
@@ -163,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="1" shapeId="0">
+    <comment ref="F25" authorId="1">
       <text>
         <r>
           <rPr>
@@ -176,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="0" shapeId="0">
+    <comment ref="A28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0">
+    <comment ref="A29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0">
+    <comment ref="A37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -240,14 +235,14 @@
     <author>ZHANG Wei AG</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>ZHANG Wei AG:</t>
         </r>
@@ -255,7 +250,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -272,7 +267,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>coll</t>
         </r>
@@ -288,7 +283,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>10</t>
         </r>
@@ -304,7 +299,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="134"/>
           </rPr>
           <t>+10</t>
         </r>
@@ -328,7 +323,7 @@
     <author>Ada</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -363,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -412,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153">
   <si>
     <t>rc</t>
   </si>
@@ -1122,12 +1117,15 @@
     <t>10560~10590</t>
   </si>
   <si>
-    <t>impeach_dealer</t>
+    <t>impeach_state</t>
   </si>
   <si>
     <t>10590~10610</t>
   </si>
   <si>
+    <t>记录impeach状态或者处理人的变化，以便形成历史记录（只有create/search，无update和delete）</t>
+  </si>
+  <si>
     <t>impeach_image</t>
   </si>
   <si>
@@ -1280,6 +1278,9 @@
     <t>50300~50400</t>
   </si>
   <si>
+    <t>uploadFile</t>
+  </si>
+  <si>
     <t>50400~50500</t>
   </si>
   <si>
@@ -1289,6 +1290,135 @@
     <t>50500~50600</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50700</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>507</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>508</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>00~50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>50900~51000</t>
+  </si>
+  <si>
     <t>redis</t>
   </si>
   <si>
@@ -1299,134 +1429,19 @@
   </si>
   <si>
     <t>30000~31000</t>
-  </si>
-  <si>
-    <t>impeach</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>uploadFile</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50700</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>507</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>508</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>00~50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1454,44 +1469,352 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1499,19 +1822,261 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1523,19 +2088,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1864,36 +2472,36 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.36328125" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" customWidth="1"/>
-    <col min="4" max="4" width="29.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="42.6328125" customWidth="1"/>
+    <col min="1" max="1" width="30.3666666666667" customWidth="1"/>
+    <col min="2" max="2" width="12.6333333333333" customWidth="1"/>
+    <col min="3" max="3" width="17.0916666666667" customWidth="1"/>
+    <col min="4" max="4" width="29.3666666666667" customWidth="1"/>
+    <col min="5" max="5" width="12.6333333333333" customWidth="1"/>
+    <col min="6" max="6" width="42.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -1903,42 +2511,42 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="4" customFormat="1" spans="2:4">
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -1947,7 +2555,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="4" customFormat="1" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1956,75 +2564,75 @@
       </c>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="3:3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" ht="14.15" customHeight="1" spans="2:4">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+    <row r="13" ht="14.15" customHeight="1" spans="2:4">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+    <row r="14" ht="14.15" customHeight="1" spans="2:4">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+    <row r="18" spans="2:6">
+      <c r="B18" s="2"/>
       <c r="C18" t="s">
         <v>28</v>
       </c>
@@ -2035,52 +2643,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+    <row r="19" spans="2:2">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="2"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>70000</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" s="3" customFormat="1" spans="1:3">
+      <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="5">
@@ -2088,12 +2699,12 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
@@ -2101,7 +2712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
@@ -2109,7 +2720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -2117,7 +2728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2125,7 +2736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2134,27 +2745,28 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.9083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2162,7 +2774,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -2171,71 +2783,72 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:D41"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.2666666666667" customWidth="1"/>
+    <col min="2" max="2" width="27.0916666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:3">
+      <c r="B3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:3">
+      <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:3">
+      <c r="B5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:3">
+      <c r="B6" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:4">
+      <c r="B7" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -2245,22 +2858,22 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+    <row r="8" spans="2:3">
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" ht="12.75" customHeight="1" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
         <v>63</v>
       </c>
@@ -2268,7 +2881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
         <v>65</v>
       </c>
@@ -2276,7 +2889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -2284,7 +2897,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>69</v>
       </c>
@@ -2292,7 +2905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -2300,7 +2913,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -2308,11 +2921,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="19" ht="12.75" customHeight="1"/>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -2323,7 +2936,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>78</v>
       </c>
@@ -2331,7 +2944,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>80</v>
       </c>
@@ -2339,7 +2952,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>82</v>
       </c>
@@ -2347,7 +2960,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>84</v>
       </c>
@@ -2355,7 +2968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>86</v>
       </c>
@@ -2363,7 +2976,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -2374,7 +2987,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>90</v>
       </c>
@@ -2382,237 +2995,242 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" t="s">
         <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.45" customWidth="1"/>
+    <col min="2" max="2" width="17.2666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.725" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
+    <col min="2" max="3" width="11.45" customWidth="1"/>
+    <col min="4" max="4" width="22.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4">
       <c r="C3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
       <c r="D4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2620,15 +3238,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2636,93 +3254,102 @@
         <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C25" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>147</v>
       </c>
-      <c r="C21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" t="s">
-        <v>146</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="C28" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>